<commit_message>
start st.gallen and update recruitment
</commit_message>
<xml_diff>
--- a/RETUNE_recruitment.xlsx
+++ b/RETUNE_recruitment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usbch.sharepoint.com/teams/c0620/Freigegebene Dokumente/RETUNE/18_website/RETUNE_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D529C1F-6754-744C-BDB3-95C274752AB7}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58700AB9-C018-494E-817D-E0D26688503A}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="500" windowWidth="38420" windowHeight="24940" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
+    <workbookView xWindow="4880" yWindow="760" windowWidth="25800" windowHeight="16960" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Zuerich</t>
+  </si>
+  <si>
+    <t>St.Gallen</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFC9B8A-85DD-B049-AB11-35BA14E37F74}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1067,6 +1070,99 @@
         <v>1</v>
       </c>
     </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45812</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45812</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H46">
     <sortCondition ref="A2:A46"/>
@@ -1076,28 +1172,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Confidentiality xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">Intern</Confidentiality>
-    <Patientdata xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">false</Patientdata>
-    <TaxCatchAll xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c57b41f-cbf4-457f-bf80-bd53c8e26310">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="USB-Dokument" ma:contentTypeID="0x01010074254FFFFA788748BE9570FD90FA56DE00A6BA077A5C2D0748B0D413E1B37C0DF4" ma:contentTypeVersion="19" ma:contentTypeDescription="Ein neues USB-Dokument in der Bibliothek erstellen." ma:contentTypeScope="" ma:versionID="0460c219e33ceaadeeb1895857d9b3d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee2de805-d424-449f-84ad-9da0e2dd7d39" xmlns:ns3="4c57b41f-cbf4-457f-bf80-bd53c8e26310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98253a3e49edcf8b82886c2b64617efc" ns2:_="" ns3:_="">
     <xsd:import namespace="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
@@ -1314,32 +1388,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0DBF876-E745-42DF-BD17-181B14022097}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Confidentiality xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">Intern</Confidentiality>
+    <Patientdata xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">false</Patientdata>
+    <TaxCatchAll xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c57b41f-cbf4-457f-bf80-bd53c8e26310">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A15F151-5EBE-4D0B-B864-B75D59C5D0EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1356,4 +1427,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
+    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0DBF876-E745-42DF-BD17-181B14022097}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add of matrial for new centers
</commit_message>
<xml_diff>
--- a/RETUNE_recruitment.xlsx
+++ b/RETUNE_recruitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usbch.sharepoint.com/teams/c0620/Freigegebene Dokumente/RETUNE/18_website/RETUNE_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{434AF06C-937C-CD47-84A2-97ED4E4B4E4F}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A58E4EB-3570-DA48-A73C-AF259F2FC982}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="760" windowWidth="25800" windowHeight="16960" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
+    <workbookView xWindow="56080" yWindow="500" windowWidth="45020" windowHeight="28300" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>St.Gallen</t>
+  </si>
+  <si>
+    <t>St. Gallen</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFC9B8A-85DD-B049-AB11-35BA14E37F74}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,9 +1114,6 @@
       <c r="B49" t="s">
         <v>10</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
       <c r="H49">
         <v>1</v>
       </c>
@@ -1161,6 +1161,62 @@
       </c>
       <c r="E52">
         <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45818</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45819</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1440,16 +1496,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update recruitment and team and centers
</commit_message>
<xml_diff>
--- a/RETUNE_recruitment.xlsx
+++ b/RETUNE_recruitment.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usbch.sharepoint.com/teams/c0620/Freigegebene Dokumente/RETUNE/18_website/RETUNE_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0561343-013F-494F-8542-F89670A296C0}"/>
+  <xr:revisionPtr revIDLastSave="490" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B167CD9-E958-4D4F-B62D-562BFEC94B55}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1120" windowWidth="25800" windowHeight="17100" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
+    <workbookView xWindow="6480" yWindow="720" windowWidth="40220" windowHeight="25240" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -50,32 +50,26 @@
     <t>Uptake</t>
   </si>
   <si>
-    <t>E-cigarettes</t>
-  </si>
-  <si>
-    <t>Nicotine pouches</t>
-  </si>
-  <si>
-    <t>Nicotine Patches</t>
-  </si>
-  <si>
     <t xml:space="preserve">Control </t>
   </si>
   <si>
     <t>Basel</t>
   </si>
   <si>
-    <t>Zuerich</t>
+    <t>Saint Gall</t>
   </si>
   <si>
-    <t>St.Gallen</t>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Bern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,13 +77,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,9 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -441,19 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFC9B8A-85DD-B049-AB11-35BA14E37F74}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,153 +481,135 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
+        <v>45692</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45698</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45706</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45708</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>45712</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>45709</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>45714</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>45720</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>45708</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45712</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>45721</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45721</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45728</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45728</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>45729</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>45729</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45733</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45733</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45735</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45735</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
+        <v>45736</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -623,66 +617,60 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>45736</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>45737</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>45737</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45741</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45741</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45743</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45744</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -690,38 +678,35 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45747</v>
       </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45754</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45754</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -730,12 +715,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45754</v>
       </c>
-      <c r="B21" t="s">
-        <v>8</v>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -744,45 +729,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>45755</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>45756</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>45756</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45757</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -791,76 +779,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>45764</v>
       </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>45764</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>45764</v>
       </c>
-      <c r="B28" t="s">
-        <v>8</v>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45770</v>
       </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>45771</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>45775</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -868,119 +853,107 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>45777</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45783</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45783</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45785</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45789</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>45789</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45796</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45796</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45798</v>
       </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45799</v>
       </c>
-      <c r="B40" t="s">
-        <v>8</v>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -989,12 +962,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45799</v>
       </c>
-      <c r="B41" t="s">
-        <v>9</v>
+      <c r="B41" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1003,23 +976,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45803</v>
       </c>
-      <c r="B42" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45803</v>
       </c>
-      <c r="B43" t="s">
-        <v>8</v>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1028,12 +1001,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45804</v>
       </c>
-      <c r="B44" t="s">
-        <v>8</v>
+      <c r="B44" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1041,16 +1014,13 @@
       <c r="D44">
         <v>1</v>
       </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45804</v>
       </c>
-      <c r="B45" t="s">
-        <v>9</v>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1059,23 +1029,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45805</v>
       </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45811</v>
       </c>
-      <c r="B47" t="s">
-        <v>8</v>
+      <c r="B47" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1083,16 +1053,13 @@
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45811</v>
       </c>
-      <c r="B48" t="s">
-        <v>8</v>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1100,175 +1067,514 @@
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45812</v>
       </c>
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45812</v>
       </c>
-      <c r="B50" t="s">
-        <v>8</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>45813</v>
-      </c>
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45812</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45813</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45818</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45819</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45820</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45820</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>45828</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45831</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45831</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>45832</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>45834</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>45840</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>45845</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>45845</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>45847</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>45848</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>45848</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>45852</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>45853</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>45818</v>
-      </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>45819</v>
-      </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>45824</v>
-      </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>45824</v>
-      </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>45825</v>
-      </c>
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>45826</v>
-      </c>
-      <c r="B58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>45826</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>45823</v>
-      </c>
-      <c r="H60">
-        <v>1</v>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>45838</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>45839</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>45842</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>45845</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>45846</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>45848</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>45849</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>45853</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>45853</v>
+      </c>
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H46">
-    <sortCondition ref="A2:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E71">
+    <sortCondition ref="A2:A71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1543,15 +1849,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Addition of protocol amendment history and update of recruitment numbers
</commit_message>
<xml_diff>
--- a/RETUNE_recruitment.xlsx
+++ b/RETUNE_recruitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usbch.sharepoint.com/teams/c0620/Freigegebene Dokumente/RETUNE/18_website/RETUNE_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4B8C58-52CE-9F4E-9EA1-F2C0A502CCFE}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="8_{51399C67-AD59-964E-9247-4C3D428189F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE93B2C-E260-3C41-9DBE-C3C69976FB19}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="700" windowWidth="40220" windowHeight="25240" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
+    <workbookView xWindow="4320" yWindow="740" windowWidth="40220" windowHeight="25240" xr2:uid="{1D389274-2DC7-8A41-9A7B-CCBF56013A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -126,13 +126,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -467,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFC9B8A-85DD-B049-AB11-35BA14E37F74}">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G138" sqref="G138"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J229" sqref="J229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2586,15 +2587,647 @@
         <v>1</v>
       </c>
     </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>45917</v>
+      </c>
+      <c r="B182" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>45916</v>
+      </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>45916</v>
+      </c>
+      <c r="B184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B185" t="s">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B186" t="s">
+        <v>8</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B187" t="s">
+        <v>8</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B188" t="s">
+        <v>11</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B189" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>45911</v>
+      </c>
+      <c r="B190" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>45910</v>
+      </c>
+      <c r="B191" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>45909</v>
+      </c>
+      <c r="B192" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>45908</v>
+      </c>
+      <c r="B193" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>45908</v>
+      </c>
+      <c r="B194" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>45908</v>
+      </c>
+      <c r="B195" t="s">
+        <v>8</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>45905</v>
+      </c>
+      <c r="B196" t="s">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>45904</v>
+      </c>
+      <c r="B197" t="s">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>45904</v>
+      </c>
+      <c r="B198" t="s">
+        <v>11</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>45903</v>
+      </c>
+      <c r="B199" t="s">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>45903</v>
+      </c>
+      <c r="B200" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="6">
+        <v>45902</v>
+      </c>
+      <c r="B201" t="s">
+        <v>11</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B202" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B203" t="s">
+        <v>8</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B204" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B205" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B206" t="s">
+        <v>11</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>45898</v>
+      </c>
+      <c r="B207" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>45897</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="5">
+        <v>45897</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="5">
+        <v>45898</v>
+      </c>
+      <c r="E210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="5">
+        <v>45898</v>
+      </c>
+      <c r="E211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="4">
+        <v>45904</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="5">
+        <v>45904</v>
+      </c>
+      <c r="E213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="5">
+        <v>45905</v>
+      </c>
+      <c r="E214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="5">
+        <v>45905</v>
+      </c>
+      <c r="E215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="5">
+        <v>45905</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="5">
+        <v>45905</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="5">
+        <v>45905</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="5">
+        <v>45908</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="5">
+        <v>45908</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" s="5">
+        <v>45908</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" s="5">
+        <v>45909</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" s="5">
+        <v>45909</v>
+      </c>
+      <c r="E223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="5">
+        <v>45909</v>
+      </c>
+      <c r="E224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" s="5">
+        <v>45910</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="5">
+        <v>45910</v>
+      </c>
+      <c r="E226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" s="5">
+        <v>45910</v>
+      </c>
+      <c r="E227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" s="5">
+        <v>45910</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" s="5">
+        <v>45910</v>
+      </c>
+      <c r="E229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" s="5">
+        <v>45911</v>
+      </c>
+      <c r="E230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" s="5">
+        <v>45911</v>
+      </c>
+      <c r="E231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" s="4">
+        <v>45915</v>
+      </c>
+      <c r="E232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" s="5">
+        <v>45915</v>
+      </c>
+      <c r="E233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" s="5">
+        <v>45916</v>
+      </c>
+      <c r="E234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" s="5">
+        <v>45918</v>
+      </c>
+      <c r="E235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" s="5">
+        <v>45918</v>
+      </c>
+      <c r="E236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" s="5">
+        <v>45918</v>
+      </c>
+      <c r="E237">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E71">
-    <sortCondition ref="A2:A71"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A209:A237">
+    <sortCondition ref="A209:A237"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Confidentiality xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">Intern</Confidentiality>
+    <Patientdata xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">false</Patientdata>
+    <TaxCatchAll xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c57b41f-cbf4-457f-bf80-bd53c8e26310">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="USB-Dokument" ma:contentTypeID="0x01010074254FFFFA788748BE9570FD90FA56DE00A6BA077A5C2D0748B0D413E1B37C0DF4" ma:contentTypeVersion="19" ma:contentTypeDescription="Ein neues USB-Dokument in der Bibliothek erstellen." ma:contentTypeScope="" ma:versionID="0460c219e33ceaadeeb1895857d9b3d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee2de805-d424-449f-84ad-9da0e2dd7d39" xmlns:ns3="4c57b41f-cbf4-457f-bf80-bd53c8e26310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98253a3e49edcf8b82886c2b64617efc" ns2:_="" ns3:_="">
     <xsd:import namespace="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
@@ -2811,29 +3444,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Confidentiality xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">Intern</Confidentiality>
-    <Patientdata xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39">false</Patientdata>
-    <TaxCatchAll xmlns="ee2de805-d424-449f-84ad-9da0e2dd7d39" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c57b41f-cbf4-457f-bf80-bd53c8e26310">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0DBF876-E745-42DF-BD17-181B14022097}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
+    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A15F151-5EBE-4D0B-B864-B75D59C5D0EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2850,29 +3486,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF03F65C-5CED-4A89-8A63-D9B2AEB56D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee2de805-d424-449f-84ad-9da0e2dd7d39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4c57b41f-cbf4-457f-bf80-bd53c8e26310"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0DBF876-E745-42DF-BD17-181B14022097}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>